<commit_message>
modifica dicionário de dados cadastrados
</commit_message>
<xml_diff>
--- a/Dicionario_de_Dados_Oscar.xlsx
+++ b/Dicionario_de_Dados_Oscar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F642056C-C800-492F-9920-D46924096D8E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564D1DA5-89E4-4B15-BB25-255CD649B553}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="81">
   <si>
     <t>Coluna</t>
   </si>
@@ -244,6 +244,30 @@
   </si>
   <si>
     <t>cidade do ator.</t>
+  </si>
+  <si>
+    <t>filme_premio (associativa)</t>
+  </si>
+  <si>
+    <t>id_filme_premio</t>
+  </si>
+  <si>
+    <t>ano_premio</t>
+  </si>
+  <si>
+    <t>Ano em que o prêmio foi recebido.</t>
+  </si>
+  <si>
+    <t>Referência ao filme associado.</t>
+  </si>
+  <si>
+    <t>Referência ao prêmio associado.</t>
+  </si>
+  <si>
+    <t>filme_ator (associativa)</t>
+  </si>
+  <si>
+    <t>id_filme_ator</t>
   </si>
 </sst>
 </file>
@@ -315,10 +339,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,14 +681,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="3" width="24.5703125" customWidth="1"/>
     <col min="4" max="4" width="28.28515625" customWidth="1"/>
     <col min="5" max="5" width="50.28515625" customWidth="1"/>
@@ -688,7 +714,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -705,7 +731,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
@@ -720,7 +746,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
@@ -735,7 +761,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="3" t="s">
         <v>39</v>
       </c>
@@ -750,11 +776,11 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -774,7 +800,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -791,7 +817,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
+      <c r="A9" s="5"/>
       <c r="B9" s="3" t="s">
         <v>50</v>
       </c>
@@ -806,7 +832,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+      <c r="A10" s="5"/>
       <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
@@ -821,7 +847,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+      <c r="A11" s="5"/>
       <c r="B11" s="3" t="s">
         <v>54</v>
       </c>
@@ -836,7 +862,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
+      <c r="A12" s="5"/>
       <c r="B12" s="3" t="s">
         <v>57</v>
       </c>
@@ -851,11 +877,11 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -875,7 +901,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="5" t="s">
         <v>59</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -892,7 +918,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
+      <c r="A16" s="5"/>
       <c r="B16" s="3" t="s">
         <v>62</v>
       </c>
@@ -907,7 +933,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
+      <c r="A17" s="5"/>
       <c r="B17" s="3" t="s">
         <v>63</v>
       </c>
@@ -922,7 +948,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
+      <c r="A18" s="5"/>
       <c r="B18" s="3" t="s">
         <v>39</v>
       </c>
@@ -937,11 +963,11 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -961,7 +987,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="5" t="s">
         <v>67</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -978,7 +1004,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
+      <c r="A22" s="5"/>
       <c r="B22" s="3" t="s">
         <v>50</v>
       </c>
@@ -993,7 +1019,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
+      <c r="A23" s="5"/>
       <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
@@ -1008,7 +1034,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
+      <c r="A24" s="5"/>
       <c r="B24" s="3" t="s">
         <v>54</v>
       </c>
@@ -1023,7 +1049,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
+      <c r="A25" s="5"/>
       <c r="B25" s="3" t="s">
         <v>57</v>
       </c>
@@ -1037,12 +1063,171 @@
         <v>72</v>
       </c>
     </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+      <c r="B35" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="B36" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="A34:A36"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="A21:A25"/>
+    <mergeCell ref="A28:A31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>